<commit_message>
Updated benchmarks with latest marko-widgets and React
marko-widgets now has morphdom integrated for faster DOM updates
</commit_message>
<xml_diff>
--- a/test/charts.xlsx
+++ b/test/charts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="20" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="140" yWindow="-23960" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Charts" sheetId="5" r:id="rId1"/>
@@ -300,11 +300,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2072053688"/>
-        <c:axId val="-2144940712"/>
+        <c:axId val="2117919704"/>
+        <c:axId val="2117925192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2072053688"/>
+        <c:axId val="2117919704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -333,7 +333,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144940712"/>
+        <c:crossAx val="2117925192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -341,7 +341,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144940712"/>
+        <c:axId val="2117925192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -372,7 +372,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2072053688"/>
+        <c:crossAx val="2117919704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -487,19 +487,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>71.16</c:v>
+                  <c:v>72.13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60.42</c:v>
+                  <c:v>69.71</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69.59</c:v>
+                  <c:v>76.06</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>71.19</c:v>
+                  <c:v>77.59</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>69.9</c:v>
+                  <c:v>79.65000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -530,19 +530,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>82.64</c:v>
+                  <c:v>82.99</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>97.32</c:v>
+                  <c:v>97.93</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>97.94</c:v>
+                  <c:v>98.49</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98.06</c:v>
+                  <c:v>98.53</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>97.68000000000001</c:v>
+                  <c:v>94.37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -560,11 +560,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2145550760"/>
-        <c:axId val="-2145545272"/>
+        <c:axId val="2117999176"/>
+        <c:axId val="2118004664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2145550760"/>
+        <c:axId val="2117999176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -593,7 +593,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145545272"/>
+        <c:crossAx val="2118004664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -601,7 +601,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2145545272"/>
+        <c:axId val="2118004664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -631,7 +631,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145550760"/>
+        <c:crossAx val="2117999176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -746,19 +746,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>86.0</c:v>
+                  <c:v>90.45</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88.14</c:v>
+                  <c:v>92.19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88.08</c:v>
+                  <c:v>94.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>88.68000000000001</c:v>
+                  <c:v>94.83</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>89.62</c:v>
+                  <c:v>94.69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -789,19 +789,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>93.49</c:v>
+                  <c:v>94.29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>94.37</c:v>
+                  <c:v>94.86</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>94.09</c:v>
+                  <c:v>95.54</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>93.68000000000001</c:v>
+                  <c:v>95.73</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>93.7</c:v>
+                  <c:v>95.77</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -819,11 +819,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2144847480"/>
-        <c:axId val="-2144841992"/>
+        <c:axId val="2118043656"/>
+        <c:axId val="2118049144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2144847480"/>
+        <c:axId val="2118043656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -852,7 +852,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144841992"/>
+        <c:crossAx val="2118049144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -860,7 +860,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144841992"/>
+        <c:axId val="2118049144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -890,7 +890,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144847480"/>
+        <c:crossAx val="2118043656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -997,19 +997,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.73</c:v>
+                  <c:v>2.38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.23</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.17</c:v>
+                  <c:v>3.92</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.28</c:v>
+                  <c:v>4.83</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.58</c:v>
+                  <c:v>6.39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1040,19 +1040,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>12.79</c:v>
+                  <c:v>15.24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.29</c:v>
+                  <c:v>25.81</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.59</c:v>
+                  <c:v>39.15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.56</c:v>
+                  <c:v>54.79</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.63</c:v>
+                  <c:v>69.47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1070,11 +1070,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2144803416"/>
-        <c:axId val="-2144797928"/>
+        <c:axId val="2118088024"/>
+        <c:axId val="2118093512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2144803416"/>
+        <c:axId val="2118088024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1103,7 +1103,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144797928"/>
+        <c:crossAx val="2118093512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1111,7 +1111,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144797928"/>
+        <c:axId val="2118093512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1141,7 +1141,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144803416"/>
+        <c:crossAx val="2118088024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1256,19 +1256,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>567.01</c:v>
+                  <c:v>416.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>889.79</c:v>
+                  <c:v>710.35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>935.04</c:v>
+                  <c:v>759.97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>927.95</c:v>
+                  <c:v>821.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>886.34</c:v>
+                  <c:v>778.0599999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1299,19 +1299,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>78.06</c:v>
+                  <c:v>65.49</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98.38</c:v>
+                  <c:v>77.34</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>97.79</c:v>
+                  <c:v>76.45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98.27</c:v>
+                  <c:v>72.76</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>98.33</c:v>
+                  <c:v>71.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1329,11 +1329,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2144758792"/>
-        <c:axId val="-2144753352"/>
+        <c:axId val="2117345640"/>
+        <c:axId val="2117340136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2144758792"/>
+        <c:axId val="2117345640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1362,7 +1362,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144753352"/>
+        <c:crossAx val="2117340136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1370,7 +1370,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144753352"/>
+        <c:axId val="2117340136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1400,7 +1400,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144758792"/>
+        <c:crossAx val="2117345640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1927,8 +1927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S15" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1973,10 +1973,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1.73</v>
+        <v>2.38</v>
       </c>
       <c r="C2">
-        <v>12.79</v>
+        <v>15.24</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1984,10 +1984,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2.23</v>
+        <v>2.8</v>
       </c>
       <c r="C3">
-        <v>20.29</v>
+        <v>25.81</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1995,10 +1995,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3.17</v>
+        <v>3.92</v>
       </c>
       <c r="C4">
-        <v>30.59</v>
+        <v>39.15</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2006,10 +2006,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4.28</v>
+        <v>4.83</v>
       </c>
       <c r="C5">
-        <v>40.56</v>
+        <v>54.79</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2017,10 +2017,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5.58</v>
+        <v>6.39</v>
       </c>
       <c r="C6">
-        <v>50.63</v>
+        <v>69.47</v>
       </c>
     </row>
   </sheetData>
@@ -2062,10 +2062,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>567.01</v>
+        <v>416.4</v>
       </c>
       <c r="C2">
-        <v>78.06</v>
+        <v>65.489999999999995</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2073,10 +2073,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>889.79</v>
+        <v>710.35</v>
       </c>
       <c r="C3">
-        <v>98.38</v>
+        <v>77.34</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2084,10 +2084,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>935.04</v>
+        <v>759.97</v>
       </c>
       <c r="C4">
-        <v>97.79</v>
+        <v>76.45</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2095,10 +2095,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>927.95</v>
+        <v>821.8</v>
       </c>
       <c r="C5">
-        <v>98.27</v>
+        <v>72.760000000000005</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2106,10 +2106,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>886.34</v>
+        <v>778.06</v>
       </c>
       <c r="C6">
-        <v>98.33</v>
+        <v>71.67</v>
       </c>
     </row>
   </sheetData>
@@ -2153,10 +2153,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>71.16</v>
+        <v>72.13</v>
       </c>
       <c r="C2">
-        <v>82.64</v>
+        <v>82.99</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2164,10 +2164,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>60.42</v>
+        <v>69.709999999999994</v>
       </c>
       <c r="C3">
-        <v>97.32</v>
+        <v>97.93</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2175,10 +2175,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>69.59</v>
+        <v>76.06</v>
       </c>
       <c r="C4">
-        <v>97.94</v>
+        <v>98.49</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2186,10 +2186,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>71.19</v>
+        <v>77.59</v>
       </c>
       <c r="C5">
-        <v>98.06</v>
+        <v>98.53</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2197,10 +2197,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>69.900000000000006</v>
+        <v>79.650000000000006</v>
       </c>
       <c r="C6">
-        <v>97.68</v>
+        <v>94.37</v>
       </c>
     </row>
   </sheetData>
@@ -2242,10 +2242,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>86</v>
+        <v>90.45</v>
       </c>
       <c r="C2">
-        <v>93.49</v>
+        <v>94.29</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2253,10 +2253,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>88.14</v>
+        <v>92.19</v>
       </c>
       <c r="C3">
-        <v>94.37</v>
+        <v>94.86</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2264,10 +2264,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>88.08</v>
+        <v>94.3</v>
       </c>
       <c r="C4">
-        <v>94.09</v>
+        <v>95.54</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2275,10 +2275,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>88.68</v>
+        <v>94.83</v>
       </c>
       <c r="C5">
-        <v>93.68</v>
+        <v>95.73</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2286,10 +2286,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>89.62</v>
+        <v>94.69</v>
       </c>
       <c r="C6">
-        <v>93.7</v>
+        <v>95.77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upgraded to latest versions and updates results
</commit_message>
<xml_diff>
--- a/test/charts.xlsx
+++ b/test/charts.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psteeleidem/development/github/patrick-steele-idem/marko-vs-react/test/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="140" yWindow="-23960" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="140" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Charts" sheetId="5" r:id="rId1"/>
@@ -31,7 +36,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="cpu.csv" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
-    <textPr prompt="0" fileType="mac" sourceFile="Macintosh HD:Users:psteeleidem:development:github:patrick-steele-idem:marko-vs-react:test:generated:cpu.csv" comma="1">
+    <textPr prompt="0" fileType="mac" sourceFile="/Users/psteeleidem/development/github/patrick-steele-idem/marko-vs-react/test/generated/cpu.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -40,7 +45,7 @@
     </textPr>
   </connection>
   <connection id="2" name="memory.csv" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
-    <textPr prompt="0" fileType="mac" sourceFile="Macintosh HD:Users:psteeleidem:development:github:patrick-steele-idem:marko-vs-react:test:generated:memory.csv" comma="1">
+    <textPr prompt="0" fileType="mac" sourceFile="/Users/psteeleidem/development/github/patrick-steele-idem/marko-vs-react/test/generated/memory.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
@@ -74,7 +79,7 @@
     </textPr>
   </connection>
   <connection id="6" name="requestsPerSecond.csv3" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
-    <textPr prompt="0" fileType="mac" sourceFile="Macintosh HD:Users:psteeleidem:development:github:patrick-steele-idem:marko-vs-react:test:generated:requestsPerSecond.csv" comma="1">
+    <textPr prompt="0" fileType="mac" sourceFile="/Users/psteeleidem/development/github/patrick-steele-idem/marko-vs-react/test/generated/requestsPerSecond.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -83,7 +88,7 @@
     </textPr>
   </connection>
   <connection id="7" name="responseTime.csv" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
-    <textPr prompt="0" fileType="mac" sourceFile="Macintosh HD:Users:psteeleidem:development:github:patrick-steele-idem:marko-vs-react:test:generated:responseTime.csv" comma="1">
+    <textPr prompt="0" fileType="mac" sourceFile="/Users/psteeleidem/development/github/patrick-steele-idem/marko-vs-react/test/generated/responseTime.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -171,230 +176,15 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Average Requests per</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Second</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>(higher is better)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>#REF!</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>#REF!</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>#REF!</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>#REF!</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>#REF!</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>#REF!</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:dLblPos val="t"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="2117919704"/>
-        <c:axId val="2117925192"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="2117919704"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Concurrency</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117925192"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2117925192"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Requests per second</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" baseline="0"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117919704"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -480,6 +270,29 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>cpuUsage!$B$2:$B$6</c:f>
@@ -487,19 +300,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>72.13</c:v>
+                  <c:v>68.97</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>69.71</c:v>
+                  <c:v>59.64</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>76.06</c:v>
+                  <c:v>71.39</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>77.59</c:v>
+                  <c:v>71.24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79.65000000000001</c:v>
+                  <c:v>75.61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -523,6 +336,29 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>cpuUsage!$C$2:$C$6</c:f>
@@ -530,19 +366,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>82.99</c:v>
+                  <c:v>79.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>97.93</c:v>
+                  <c:v>95.43</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98.49</c:v>
+                  <c:v>97.04</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98.53</c:v>
+                  <c:v>97.11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>94.37</c:v>
+                  <c:v>96.89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -558,13 +394,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2117999176"/>
-        <c:axId val="2118004664"/>
+        <c:axId val="-2121998800"/>
+        <c:axId val="-2122003536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2117999176"/>
+        <c:axId val="-2121998800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -593,7 +428,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118004664"/>
+        <c:crossAx val="-2122003536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -601,7 +436,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2118004664"/>
+        <c:axId val="-2122003536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -631,7 +466,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117999176"/>
+        <c:crossAx val="-2121998800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -653,7 +488,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -739,6 +574,29 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>memoryUsage!$B$2:$B$6</c:f>
@@ -746,19 +604,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>90.45</c:v>
+                  <c:v>145.27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>92.19</c:v>
+                  <c:v>202.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>94.3</c:v>
+                  <c:v>215.62</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>94.83</c:v>
+                  <c:v>213.82</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>94.69</c:v>
+                  <c:v>232.31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -782,6 +640,29 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>memoryUsage!$C$2:$C$6</c:f>
@@ -789,19 +670,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>94.29</c:v>
+                  <c:v>185.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>94.86</c:v>
+                  <c:v>214.91</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>95.54</c:v>
+                  <c:v>223.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>95.73</c:v>
+                  <c:v>214.11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>95.77</c:v>
+                  <c:v>201.88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -817,13 +698,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2118043656"/>
-        <c:axId val="2118049144"/>
+        <c:axId val="-2122088512"/>
+        <c:axId val="-2122093056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2118043656"/>
+        <c:axId val="-2122088512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -852,7 +732,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118049144"/>
+        <c:crossAx val="-2122093056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -860,7 +740,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2118049144"/>
+        <c:axId val="-2122093056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -890,7 +770,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118043656"/>
+        <c:crossAx val="-2122088512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -912,7 +792,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -990,6 +870,29 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>responseTime!$B$2:$B$6</c:f>
@@ -997,19 +900,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.38</c:v>
+                  <c:v>2.51</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8</c:v>
+                  <c:v>2.85</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.92</c:v>
+                  <c:v>3.82</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.83</c:v>
+                  <c:v>4.71</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.39</c:v>
+                  <c:v>6.14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1033,6 +936,29 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>responseTime!$C$2:$C$6</c:f>
@@ -1040,19 +966,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>15.24</c:v>
+                  <c:v>9.11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.81</c:v>
+                  <c:v>12.92</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.15</c:v>
+                  <c:v>18.93</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54.79</c:v>
+                  <c:v>25.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>69.47</c:v>
+                  <c:v>31.42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1068,13 +994,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2118088024"/>
-        <c:axId val="2118093512"/>
+        <c:axId val="-2122134288"/>
+        <c:axId val="-2122138784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2118088024"/>
+        <c:axId val="-2122134288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1103,7 +1028,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118093512"/>
+        <c:crossAx val="-2122138784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1111,7 +1036,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2118093512"/>
+        <c:axId val="-2122138784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1141,7 +1066,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118088024"/>
+        <c:crossAx val="-2122134288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1163,7 +1088,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1249,6 +1174,29 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>requestsPerSecond!$B$2:$B$6</c:f>
@@ -1256,19 +1204,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>416.4</c:v>
+                  <c:v>392.72</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>710.35</c:v>
+                  <c:v>696.71</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>759.97</c:v>
+                  <c:v>781.12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>821.8</c:v>
+                  <c:v>843.68</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>778.0599999999999</c:v>
+                  <c:v>808.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1292,6 +1240,29 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>requestsPerSecond!$C$2:$C$6</c:f>
@@ -1299,19 +1270,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>65.49</c:v>
+                  <c:v>109.46</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>77.34</c:v>
+                  <c:v>154.39</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>76.45</c:v>
+                  <c:v>157.99</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>72.76</c:v>
+                  <c:v>158.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>71.67</c:v>
+                  <c:v>158.31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1327,13 +1298,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2117345640"/>
-        <c:axId val="2117340136"/>
+        <c:axId val="-2122180896"/>
+        <c:axId val="-2122185456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2117345640"/>
+        <c:axId val="-2122180896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1362,7 +1332,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117340136"/>
+        <c:crossAx val="-2122185456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1370,7 +1340,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117340136"/>
+        <c:axId val="-2122185456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1400,7 +1370,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117345640"/>
+        <c:crossAx val="-2122180896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1424,38 +1394,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>132080</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1482,7 +1420,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1514,7 +1452,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1546,7 +1484,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1578,7 +1516,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1588,19 +1526,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="responseTime" refreshOnLoad="1" connectionId="7" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="responseTime" refreshOnLoad="1" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="requestsPerSecond" refreshOnLoad="1" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="requestsPerSecond" refreshOnLoad="1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cpu" refreshOnLoad="1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cpu" refreshOnLoad="1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="memory" refreshOnLoad="1" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="memory" refreshOnLoad="1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1927,20 +1865,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1950,14 +1883,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1968,68 +1901,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2.38</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="C2">
-        <v>15.24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>9.11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2.8</v>
+        <v>2.85</v>
       </c>
       <c r="C3">
-        <v>25.81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>12.92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3.92</v>
+        <v>3.82</v>
       </c>
       <c r="C4">
-        <v>39.15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>18.93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4.83</v>
+        <v>4.71</v>
       </c>
       <c r="C5">
-        <v>54.79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>25.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>6.39</v>
+        <v>6.14</v>
       </c>
       <c r="C6">
-        <v>69.47</v>
+        <v>31.42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2039,14 +1967,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2057,68 +1984,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>416.4</v>
+        <v>392.72</v>
       </c>
       <c r="C2">
-        <v>65.489999999999995</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>109.46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>710.35</v>
+        <v>696.71</v>
       </c>
       <c r="C3">
-        <v>77.34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>154.38999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>759.97</v>
+        <v>781.12</v>
       </c>
       <c r="C4">
-        <v>76.45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>157.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>821.8</v>
+        <v>843.68</v>
       </c>
       <c r="C5">
-        <v>72.760000000000005</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>158.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>778.06</v>
+        <v>808.1</v>
       </c>
       <c r="C6">
-        <v>71.67</v>
+        <v>158.31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2130,14 +2052,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2148,68 +2070,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>72.13</v>
+        <v>68.97</v>
       </c>
       <c r="C2">
-        <v>82.99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>79.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>69.709999999999994</v>
+        <v>59.64</v>
       </c>
       <c r="C3">
-        <v>97.93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>95.43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>76.06</v>
+        <v>71.39</v>
       </c>
       <c r="C4">
-        <v>98.49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>97.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>77.59</v>
+        <v>71.239999999999995</v>
       </c>
       <c r="C5">
-        <v>98.53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>97.11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>79.650000000000006</v>
+        <v>75.61</v>
       </c>
       <c r="C6">
-        <v>94.37</v>
+        <v>96.89</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2217,16 +2134,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2237,67 +2155,62 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>90.45</v>
+        <v>145.27000000000001</v>
       </c>
       <c r="C2">
-        <v>94.29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>185.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>92.19</v>
+        <v>202.8</v>
       </c>
       <c r="C3">
-        <v>94.86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>214.91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>94.3</v>
+        <v>215.62</v>
       </c>
       <c r="C4">
-        <v>95.54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>223.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>94.83</v>
+        <v>213.82</v>
       </c>
       <c r="C5">
-        <v>95.73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>214.11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>94.69</v>
+        <v>232.31</v>
       </c>
       <c r="C6">
-        <v>95.77</v>
+        <v>201.88</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated to Marko v4
</commit_message>
<xml_diff>
--- a/test/charts.xlsx
+++ b/test/charts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27815"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="140" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="140" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Charts" sheetId="5" r:id="rId1"/>
@@ -26,6 +26,9 @@
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -300,19 +303,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>68.97</c:v>
+                  <c:v>71.09</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59.64</c:v>
+                  <c:v>62.85</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71.39</c:v>
+                  <c:v>71.81</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>71.24</c:v>
+                  <c:v>69.87</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>75.61</c:v>
+                  <c:v>67.42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -366,19 +369,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>79.3</c:v>
+                  <c:v>79.95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>95.43</c:v>
+                  <c:v>94.57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>97.04</c:v>
+                  <c:v>97.93</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>97.11</c:v>
+                  <c:v>96.96</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>96.89</c:v>
+                  <c:v>97.76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -395,11 +398,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2121998800"/>
-        <c:axId val="-2122003536"/>
+        <c:axId val="-949214096"/>
+        <c:axId val="-949207184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2121998800"/>
+        <c:axId val="-949214096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -428,7 +431,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122003536"/>
+        <c:crossAx val="-949207184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -436,7 +439,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122003536"/>
+        <c:axId val="-949207184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -466,7 +469,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121998800"/>
+        <c:crossAx val="-949214096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -604,19 +607,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>145.27</c:v>
+                  <c:v>271.44</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>202.8</c:v>
+                  <c:v>294.48</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>215.62</c:v>
+                  <c:v>224.71</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>213.82</c:v>
+                  <c:v>225.65</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>232.31</c:v>
+                  <c:v>235.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -670,19 +673,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>185.4</c:v>
+                  <c:v>230.69</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>214.91</c:v>
+                  <c:v>295.98</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>223.5</c:v>
+                  <c:v>258.43</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>214.11</c:v>
+                  <c:v>368.49</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>201.88</c:v>
+                  <c:v>263.88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -699,11 +702,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2122088512"/>
-        <c:axId val="-2122093056"/>
+        <c:axId val="-949113904"/>
+        <c:axId val="-949107424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2122088512"/>
+        <c:axId val="-949113904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -732,7 +735,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122093056"/>
+        <c:crossAx val="-949107424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -740,7 +743,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122093056"/>
+        <c:axId val="-949107424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,7 +773,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122088512"/>
+        <c:crossAx val="-949113904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -903,16 +906,16 @@
                   <c:v>2.51</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.85</c:v>
+                  <c:v>2.81</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.82</c:v>
+                  <c:v>3.63</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.71</c:v>
+                  <c:v>4.44</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.14</c:v>
+                  <c:v>6.03</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -966,19 +969,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9.11</c:v>
+                  <c:v>9.27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.92</c:v>
+                  <c:v>12.62</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.93</c:v>
+                  <c:v>18.09</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25.1</c:v>
+                  <c:v>24.72</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31.42</c:v>
+                  <c:v>29.55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -995,11 +998,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2122134288"/>
-        <c:axId val="-2122138784"/>
+        <c:axId val="-949043440"/>
+        <c:axId val="-949036960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2122134288"/>
+        <c:axId val="-949043440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1028,7 +1031,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122138784"/>
+        <c:crossAx val="-949036960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1036,7 +1039,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122138784"/>
+        <c:axId val="-949036960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1066,7 +1069,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122134288"/>
+        <c:crossAx val="-949043440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1204,19 +1207,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>392.72</c:v>
+                  <c:v>395.03</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>696.71</c:v>
+                  <c:v>707.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>781.12</c:v>
+                  <c:v>821.9299999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>843.68</c:v>
+                  <c:v>894.12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>808.1</c:v>
+                  <c:v>824.47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1270,19 +1273,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>109.46</c:v>
+                  <c:v>107.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>154.39</c:v>
+                  <c:v>158.07</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>157.99</c:v>
+                  <c:v>165.35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>158.75</c:v>
+                  <c:v>160.93</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>158.31</c:v>
+                  <c:v>168.45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1299,11 +1302,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2122180896"/>
-        <c:axId val="-2122185456"/>
+        <c:axId val="-948955648"/>
+        <c:axId val="-948949104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2122180896"/>
+        <c:axId val="-948955648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1332,7 +1335,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122185456"/>
+        <c:crossAx val="-948949104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1340,7 +1343,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122185456"/>
+        <c:axId val="-948949104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1370,7 +1373,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122180896"/>
+        <c:crossAx val="-948955648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1865,8 +1868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1909,7 +1912,7 @@
         <v>2.5099999999999998</v>
       </c>
       <c r="C2">
-        <v>9.11</v>
+        <v>9.27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1917,10 +1920,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2.85</v>
+        <v>2.81</v>
       </c>
       <c r="C3">
-        <v>12.92</v>
+        <v>12.62</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1928,10 +1931,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3.82</v>
+        <v>3.63</v>
       </c>
       <c r="C4">
-        <v>18.93</v>
+        <v>18.09</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1939,10 +1942,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4.71</v>
+        <v>4.4400000000000004</v>
       </c>
       <c r="C5">
-        <v>25.1</v>
+        <v>24.72</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1950,10 +1953,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>6.14</v>
+        <v>6.03</v>
       </c>
       <c r="C6">
-        <v>31.42</v>
+        <v>29.55</v>
       </c>
     </row>
   </sheetData>
@@ -1989,10 +1992,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>392.72</v>
+        <v>395.03</v>
       </c>
       <c r="C2">
-        <v>109.46</v>
+        <v>107.7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2000,10 +2003,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>696.71</v>
+        <v>707.25</v>
       </c>
       <c r="C3">
-        <v>154.38999999999999</v>
+        <v>158.07</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2011,10 +2014,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>781.12</v>
+        <v>821.93</v>
       </c>
       <c r="C4">
-        <v>157.99</v>
+        <v>165.35</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2022,10 +2025,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>843.68</v>
+        <v>894.12</v>
       </c>
       <c r="C5">
-        <v>158.75</v>
+        <v>160.93</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2033,10 +2036,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>808.1</v>
+        <v>824.47</v>
       </c>
       <c r="C6">
-        <v>158.31</v>
+        <v>168.45</v>
       </c>
     </row>
   </sheetData>
@@ -2075,10 +2078,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>68.97</v>
+        <v>71.09</v>
       </c>
       <c r="C2">
-        <v>79.3</v>
+        <v>79.95</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2086,10 +2089,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>59.64</v>
+        <v>62.85</v>
       </c>
       <c r="C3">
-        <v>95.43</v>
+        <v>94.57</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2097,10 +2100,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>71.39</v>
+        <v>71.81</v>
       </c>
       <c r="C4">
-        <v>97.04</v>
+        <v>97.93</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2108,10 +2111,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>71.239999999999995</v>
+        <v>69.87</v>
       </c>
       <c r="C5">
-        <v>97.11</v>
+        <v>96.96</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2119,10 +2122,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>75.61</v>
+        <v>67.42</v>
       </c>
       <c r="C6">
-        <v>96.89</v>
+        <v>97.76</v>
       </c>
     </row>
   </sheetData>
@@ -2134,7 +2137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
@@ -2160,10 +2163,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>145.27000000000001</v>
+        <v>271.44</v>
       </c>
       <c r="C2">
-        <v>185.4</v>
+        <v>230.69</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2171,10 +2174,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>202.8</v>
+        <v>294.48</v>
       </c>
       <c r="C3">
-        <v>214.91</v>
+        <v>295.98</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2182,10 +2185,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>215.62</v>
+        <v>224.71</v>
       </c>
       <c r="C4">
-        <v>223.5</v>
+        <v>258.43</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2193,10 +2196,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>213.82</v>
+        <v>225.65</v>
       </c>
       <c r="C5">
-        <v>214.11</v>
+        <v>368.49</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2204,10 +2207,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>232.31</v>
+        <v>235.35</v>
       </c>
       <c r="C6">
-        <v>201.88</v>
+        <v>263.88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>